<commit_message>
Attendance added to DB
</commit_message>
<xml_diff>
--- a/Toto_Smart_Attendance_System/sv.xlsx
+++ b/Toto_Smart_Attendance_System/sv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Major\Toto-Smart-Attendance-System\Toto_Smart_Attendance_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AE1F1F-EF16-4725-9110-B1C3E8CF1E87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F03A701-0421-4C05-AB9A-88F02783B363}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -43,25 +43,7 @@
     <t>0827CS151088</t>
   </si>
   <si>
-    <t>0827CS151066</t>
-  </si>
-  <si>
     <t>https://drive.google.com/file/d/1k9WpTnHyEojMPNlvGzx-i-lQ8KWsysZ4/view</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1FuM_edvB-hNOtk-D3-Cdae3sK--ZxWOA/view</t>
-  </si>
-  <si>
-    <t>Rubal</t>
-  </si>
-  <si>
-    <t>Dipesh</t>
-  </si>
-  <si>
-    <t>0827CS151089</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1UZJhoX9V7_EcteK8wYy9Lyb8DGHb-9B7/view</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1ktbeT2JaWmyeazv33AyTweZWYpNCAGCH/view</t>
@@ -440,7 +422,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -467,7 +449,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -478,37 +460,23 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{DDE1FB6A-878E-4138-9394-B129152DB903}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{1F5EC7AC-C524-46FA-AC97-F0B5815EA2F9}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{DDE1FB6A-878E-4138-9394-B129152DB903}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>